<commit_message>
Add read papers and references
</commit_message>
<xml_diff>
--- a/data/lit_review.xlsx
+++ b/data/lit_review.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Key" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="140">
   <si>
     <t xml:space="preserve">Reference level</t>
   </si>
@@ -45,15 +45,15 @@
     <t xml:space="preserve">Author</t>
   </si>
   <si>
+    <t xml:space="preserve">Title</t>
+  </si>
+  <si>
     <t xml:space="preserve">Year</t>
   </si>
   <si>
     <t xml:space="preserve">PMID or DOI</t>
   </si>
   <si>
-    <t xml:space="preserve">Title</t>
-  </si>
-  <si>
     <t xml:space="preserve">Document type</t>
   </si>
   <si>
@@ -66,13 +66,10 @@
     <t xml:space="preserve">Keywords</t>
   </si>
   <si>
-    <t xml:space="preserve">Main findings</t>
-  </si>
-  <si>
     <t xml:space="preserve">Methodology</t>
   </si>
   <si>
-    <t xml:space="preserve">Summary</t>
+    <t xml:space="preserve">Summary/Main findings</t>
   </si>
   <si>
     <t xml:space="preserve">Notes</t>
@@ -81,6 +78,9 @@
     <t xml:space="preserve">Section important</t>
   </si>
   <si>
+    <t xml:space="preserve">Sub-section important</t>
+  </si>
+  <si>
     <t xml:space="preserve">Other important works</t>
   </si>
   <si>
@@ -88,15 +88,15 @@
   </si>
   <si>
     <t xml:space="preserve">Tsung-Ying Yang</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10.1016/j.jmii.2017.10.006</t>
   </si>
   <si>
     <t xml:space="preserve">Update on fosfomycin-modified genes in
 Enterobacteriaceae</t>
   </si>
   <si>
+    <t xml:space="preserve">https://doi.org/10.1016/j.jmii.2017.10.006</t>
+  </si>
+  <si>
     <t xml:space="preserve">Journal article</t>
   </si>
   <si>
@@ -106,15 +106,999 @@
     <t xml:space="preserve">fos genes</t>
   </si>
   <si>
+    <t xml:space="preserve">Fosfomycin-modified genes; fos; transposons, plasmids, insertion sequences, drug combinations</t>
+  </si>
+  <si>
     <t xml:space="preserve">NA</t>
   </si>
   <si>
-    <t xml:space="preserve">Check tables for summaries on fos gene characterisation, surr genetic elements, and drug comb</t>
+    <t xml:space="preserve">- Fosfomycin is bactericidal and targets MurA responsible for peptidoglycan synthesis
+- Fosfomycin res mech: AA sub in MurA, inactivation of GlpT and UhpT transporters, genes coding for  fosfomycin-modifying enzymes (fos)
+- fos genes in transposon elements and conjugative plasmids
+- fos genes in Enterobacteriaceae: fosA, fosA2, fosA3, fosA4, fosA5, fosA6, fosC2
+- Surr environ and possible fos transmission pathways: all fos genes except fosA2 are located in plasmids; Also observed in transposons, insertion sequences (IS), and integrons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check table 1, 2, and 3  for summaries on fos gene characterisation, surr genetic elements, and drug comb respectively</t>
   </si>
   <si>
     <t xml:space="preserve">Introduction</t>
   </si>
   <si>
+    <t xml:space="preserve">Check reference section of tables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matthew K. Thompson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diversity in fosfomycin resistance proteins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1016/j.pisc.2014.12.004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">structure of fos genes and mechanism of action</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fosA; fosB; fosX; fosfomycin inactivation</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">- Fosfomycin - bactericidal, broad-spectrum (effective against g- and g+ bacteria) - inhibit cell wall biosynthesis
+- Fosfomycin res proteins are metalloenzymes that inactivate the antibiotic by addition of nucleophiles - water, glutathione (GSH), L-cysteine, and bacillithiol (BSH) to the oxirane ring of the molecule
+- They belong to the Vicinal Oxygen Chelate (VOC) superfamily of metalloenzymes and are structurally characterised by a 3D domain-swapped arrangement of tandem βαβββ motifs
+- FosA: Mn</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2+ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">and K</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">dependent glutathione-S-tranferases in g- bacterial species - catalyse nucelophilic addition of glutathione (GSH) to carbon-1  of fosfomycin opening the epoxide ring resulting in loss of bactericidal properties
+- FosB: in g+ bacteria and catalyse the Mn</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2+ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">dependent addition of L-cysteine or bcillithiol (BSH) to carbon-1 of fosfomycin
+- FosX: Mn</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2+ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">dependent hydrolases in g- bacteria - catalyse the hydration of fosfomycin at carbon-1 forming a vicinal diol and inactivating the drug
+ </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Mechanism of inactivation of fosfomyci by the fos genes explained further </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FosB from Bacillus cereus
+Further references under discussions of specific Fos proteins </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wenya Xu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Molecular Mechanisms and Epidemiology of Fosfomycin Resistance in Staphylococcus aureus Isolated From Patients at a Teaching Hospital in China</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.3389/fmicb.2020.01290</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Research article</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">fosfomycin res in </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">S. aureus</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">S.aureus; fosfomycin resistance; nosocomial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- S. aureus is a g+ pathogenic bacteria with strong res and tolerance to harsh environs - contributes to high incidences of nosocomial infections
+- Employs various mech of fosfomycin res: fosfomycin-modifying enzymes i.e. FosA, FosB, FosC, FosD, FosX and acquisition of chromosomal mutations
+- Res mainly as a result of mutations in the uhpT, glpT and murA genes  and overexpression of efflux pump gene tet38</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">fos genes in other bacteria i.e. </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">S. aureus</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Introduction </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fosfomycin resistance in other Enterobacteriaceae; Epidemiology</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">E. coli</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">P. aeruginosa</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ESBL E.coli and K. pneumo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">fosC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">E. coli (Sho)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">MurA</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Katrin Zurfluh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mobile fosfomycin resistance genes in Enterobacteriaceae— An increasing threat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1002/mbo3.1135</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fos A alleles and plasmid types involved in their dissemination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fosA; plasmids</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check table 1 for plasmid-mediated fosA and table 2 for plasmids carrying fosA genes</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Fosfomycin res</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Fosfomycin mech and res</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">fosA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">fosfomycin-modifying genes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Nerino Allocati</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Glutathione transferases in bacteria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1111/j.1742-4658.2008.06743.x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Glutathione transferases</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lin Huang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prevalence and mechanisms of fosfomycin resistance among KPC-producing Klebsiella pneumoniae clinical isolates in China</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1016/j.ijantimicag.2020.106226</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fosfomycin res in CRKP</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Main mech of res – fosA3 (high MICs) and </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">glpT </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">mutations</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Check introduction for references </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hind Alrowais</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fosfomycin Resistance in Escherichia coli,
+Pennsylvania, USA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.3201%2Feid2111.150750</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fosA3; E. coli; plasmid; horizontal transmission </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Svetlana Pakhomova</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Structure of fosfomycin resistance protein
+FosA from transposon Tn2921</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1110%2Fps.03585004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plasmid-mediated fosA (Tn2921) structure and how it differs from a chromosomally-encoded fosA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fosA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kieran A. Milner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identification and Characterization of a Novel FosA7 Member from Fosfomycin-Resistant Escherichia coli Clinical Isolates from Canadian Hospitals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1128/AAC.00865-20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fosA;fosA3; fos A7.5; fosA8; E. coli; Canada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refer to figures when creating own for report</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Michael Biggel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Characteristics of fosA-carrying plasmids in E. coli and Klebsiella spp.
+isolates originating from food and environmental samples</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1093/jac/dkab119</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enterobacteriaceae plasmids harbouring fos genes from waste water and food chain samples in Switzerland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fos genes; fosA3; plasmids; co-selection; transposable; fosfomycin resistance; insertion sequences </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refer to table 2 for plasmid characteristics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fos genes; Epidemiology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chromosomal fosA gene; KP carrying plasmid with fosA3;
+Acquired fosfomycin res in E. coli and KP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dong Wang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comparison of the prevalence and molecular characteristics of fosA3 and fosA7 among Salmonella isolates from food animals in China</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1093/jac/dkac061</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Characteristics of fosA3 and fosA7 in Salmonella isolates </t>
+  </si>
+  <si>
+    <t xml:space="preserve">fosA3; fosA7; Salmonella; chromosome; plasmid; insertion sequence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refer to figure 2 when creating figures for phylogenetic analysis results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qinglan Guo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Glutathione-S-transferase FosA6 of Klebsiella pneumoniae origin conferring fosfomycin resistance in ESBL-producing Escherichia coli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1093/jac/dkw177</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fosA6 of K. pneumoniae origin in E.coli clinical isolates carrying CTX-M </t>
+  </si>
+  <si>
+    <t xml:space="preserve">fosA6; plasmids; E.coli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shows transfer of fos genes from K. pneumo to E. coli (K. pneumo acting as  reservoir)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fosfomycin resistance in other Enterobacteriaceae</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">E.coli fosA3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">E. coli fos gene epidemiology</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">fosA5 E. coli</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">in vitro fosfomycin activity in Kp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> ; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Kp MIC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> ; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">in vitro fosfomycin activity in E.coli</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> ; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">fosfomycin against g- non-urinary pathogens</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> ; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">fosfomycin AST</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> ; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">detection of fos genes</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Muhammad A. Rehman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First Detection of a Fosfomycin Resistance Gene, fosA7, in Salmonella enterica Serovar Heidelberg Isolated from Broiler Chickens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1128/AAC.00410-17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fosA7 which was first discovered in Salmonella enterica serovar Heidelberg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fosA7; chromosome; Salmonella Heidelberg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check reviews 8-14 for fos genes, 7 and 23 for fosA3, 5 and 23 for fosA3 &amp; CTX-M,  </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">fos genes in Salmonella enterica serovar Heidelberg</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> ; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">fosfomycin res in Enterobacteriaceae</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Erik H. Klontz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Structure and Dynamics of FosA-Mediated Fosfomycin Resistance in Klebsiella pneumoniae and Escherichia coli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1128/AAC.01572-17</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Structure, molecular dynamics, catalytic activity, and fosfomycin resistance of FosA3 and FosA</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">KP</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">fosA3; fosA</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">KP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">; fosA inhibition; active site; dimer interface loops</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Check figures for structure of fosA3 and fosA</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">KP </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Regioselectivity and Chemoselectivity in FosA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">chromosomal fosA genes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">fosA5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">FosA from transposon Tn2921 structure</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">FosA active site residues</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Genki Nakamura</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Practical Agar-Based Disk Potentiation Test for Detection of Fosfomycin-Nonsusceptible Escherichia coli Clinical Isolates Producing Glutathione S-Transferases</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://dx.doi.org/10.1128/JCM.01094-14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disk potentiation test using PPF to test for the presence of glutathione S-transferases i.e. fos genes in E. coli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fosA3; fosA4, fosC2; disk potentiation test; phosphonoformate (PPF); G6P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">References for FosA3 producers in E. coli isolates from clinical specimens (7), healthy individuals (6), consumable animal products (8, 9), and domestic animals (10)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PPF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y. Ma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Characterization of fosA5, a new plasmid-mediated
+fosfomycin resistance gene in Escherichia coli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1111/lam.12366</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Discovery of novel fosA5 gene in E. coli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fosA5; E. coli; fosfomycin resistance</t>
+  </si>
+  <si>
     <t xml:space="preserve">fos gene</t>
   </si>
   <si>
@@ -140,19 +1124,17 @@
   </si>
   <si>
     <t xml:space="preserve">Shared identity with fosA (%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fosA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -194,6 +1176,20 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -204,29 +1200,36 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FF993300"/>
+        <fgColor rgb="FFFFA6A6"/>
+        <bgColor rgb="FFFFCC99"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFFFFFA6"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF81D41A"/>
-        <bgColor rgb="FF969696"/>
+        <fgColor rgb="FFB7B3CA"/>
+        <bgColor rgb="FFCCCCFF"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
@@ -255,7 +1258,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -281,18 +1284,46 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -321,7 +1352,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FFB7B3CA"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -342,14 +1373,14 @@
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FFFFFFA6"/>
       <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFFFA6A6"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF81D41A"/>
+      <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
@@ -376,7 +1407,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
+      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -429,82 +1460,85 @@
   </sheetPr>
   <dimension ref="A1:AMJ27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="K17" activeCellId="0" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="5.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="6" width="17.36"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="6" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="6" width="26.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="6" width="39.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="6" width="39.04"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="6" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="6" width="26.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="6" width="14.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="6" width="13.75"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="6" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="6" width="25.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="6" width="16.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="6" width="25.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="6" width="28.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="6" width="16.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="6" width="22.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="6" width="22.92"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="17" style="6" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="6" width="23.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="6" width="19.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="6" width="16.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="6" width="37.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="6" width="28.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="6" width="16.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="6" width="20.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="6" width="45.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="7" width="22.92"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="17" style="6" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
+    <row r="1" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="N1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="O1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="P1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="AMJ1" s="6"/>
-    </row>
-    <row r="2" customFormat="false" ht="30.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AMJ1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="127.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="n">
         <f aca="false">ROW(A1)</f>
         <v>1</v>
@@ -512,13 +1546,13 @@
       <c r="B2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="6" t="n">
+      <c r="C2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="6" t="n">
         <v>2017</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="10" t="s">
         <v>23</v>
       </c>
       <c r="F2" s="6" t="s">
@@ -530,106 +1564,660 @@
       <c r="H2" s="6" t="s">
         <v>26</v>
       </c>
+      <c r="I2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="K2" s="6" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="P2" s="9"/>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>26</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" s="11"/>
+    </row>
+    <row r="3" customFormat="false" ht="234.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="n">
         <f aca="false">ROW(A2)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="6" t="n">
+        <v>2014</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="O3" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="P3" s="11"/>
+    </row>
+    <row r="4" customFormat="false" ht="98.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="n">
         <f aca="false">ROW(A3)</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="6" t="n">
+        <v>2020</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="O4" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="P4" s="13"/>
+    </row>
+    <row r="5" customFormat="false" ht="30.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="n">
         <f aca="false">ROW(A4)</f>
         <v>4</v>
       </c>
+      <c r="B5" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="6" t="n">
+        <v>2020</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="O5" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="P5" s="11"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="n">
         <f aca="false">ROW(A5)</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" s="6" t="n">
+        <v>2008</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="P6" s="13"/>
+    </row>
+    <row r="7" customFormat="false" ht="30.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="n">
         <f aca="false">ROW(A6)</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="6" t="n">
+        <v>2020</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="P7" s="14"/>
+    </row>
+    <row r="8" customFormat="false" ht="30.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="n">
         <f aca="false">ROW(A7)</f>
         <v>7</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" s="6" t="n">
+        <v>2015</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="N8" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="P8" s="14"/>
+    </row>
+    <row r="9" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="n">
         <f aca="false">ROW(A8)</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" s="6" t="n">
+        <v>2004</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="P9" s="13"/>
+    </row>
+    <row r="10" customFormat="false" ht="30.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="n">
         <f aca="false">ROW(A9)</f>
         <v>9</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" s="6" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="N10" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="P10" s="14"/>
+    </row>
+    <row r="11" customFormat="false" ht="49.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="n">
         <f aca="false">ROW(A10)</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D11" s="6" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="N11" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="O11" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="30.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="n">
         <f aca="false">ROW(A11)</f>
         <v>11</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D12" s="6" t="n">
+        <v>2022</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="M12" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="P12" s="13"/>
+    </row>
+    <row r="13" customFormat="false" ht="49.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="n">
         <f aca="false">ROW(A12)</f>
         <v>12</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D13" s="6" t="n">
+        <v>2016</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="L13" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="N13" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="O13" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="P13" s="11"/>
+    </row>
+    <row r="14" customFormat="false" ht="30.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="n">
         <f aca="false">ROW(A13)</f>
         <v>13</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D14" s="6" t="n">
+        <v>2017</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="L14" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="M14" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N14" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="O14" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="P14" s="11"/>
+    </row>
+    <row r="15" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="n">
         <f aca="false">ROW(A14)</f>
         <v>14</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D15" s="6" t="n">
+        <v>2017</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="M15" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N15" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="O15" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="P15" s="11"/>
+    </row>
+    <row r="16" customFormat="false" ht="49.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="n">
         <f aca="false">ROW(A15)</f>
         <v>15</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D16" s="6" t="n">
+        <v>2014</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="L16" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="M16" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N16" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="O16" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="P16" s="11"/>
+    </row>
+    <row r="17" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="n">
         <f aca="false">ROW(A16)</f>
         <v>16</v>
       </c>
+      <c r="B17" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D17" s="6" t="n">
+        <v>2014</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="M17" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N17" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="P17" s="11"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="n">
@@ -693,7 +2281,24 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="10.1016/j.jmii.2017.10.006"/>
+    <hyperlink ref="E2" r:id="rId1" display="https://doi.org/10.1016/j.jmii.2017.10.006"/>
+    <hyperlink ref="E3" r:id="rId2" display="https://doi.org/10.1016/j.pisc.2014.12.004"/>
+    <hyperlink ref="O3" r:id="rId3" display="FosB from Bacillus cereus&#10;Further references under discussions of specific Fos proteins "/>
+    <hyperlink ref="E4" r:id="rId4" display="https://doi.org/10.3389/fmicb.2020.01290"/>
+    <hyperlink ref="E5" r:id="rId5" display="https://doi.org/10.1002/mbo3.1135"/>
+    <hyperlink ref="E6" r:id="rId6" display="https://doi.org/10.1111/j.1742-4658.2008.06743.x"/>
+    <hyperlink ref="E7" r:id="rId7" display="https://doi.org/10.1016/j.ijantimicag.2020.106226"/>
+    <hyperlink ref="E8" r:id="rId8" display="https://doi.org/10.3201%2Feid2111.150750"/>
+    <hyperlink ref="E9" r:id="rId9" display="https://doi.org/10.1110%2Fps.03585004"/>
+    <hyperlink ref="E10" r:id="rId10" display="https://doi.org/10.1128/AAC.00865-20"/>
+    <hyperlink ref="E11" r:id="rId11" display="https://doi.org/10.1093/jac/dkab119"/>
+    <hyperlink ref="E12" r:id="rId12" display="https://doi.org/10.1093/jac/dkac061"/>
+    <hyperlink ref="E13" r:id="rId13" display="https://doi.org/10.1093/jac/dkw177"/>
+    <hyperlink ref="E14" r:id="rId14" display="https://doi.org/10.1128/AAC.00410-17"/>
+    <hyperlink ref="E15" r:id="rId15" display="https://doi.org/10.1128/AAC.01572-17"/>
+    <hyperlink ref="E16" r:id="rId16" display="http://dx.doi.org/10.1128/JCM.01094-14"/>
+    <hyperlink ref="O16" r:id="rId17" display="PPF"/>
+    <hyperlink ref="E17" r:id="rId18" display="https://doi.org/10.1111/lam.12366"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -712,60 +2317,60 @@
   </sheetPr>
   <dimension ref="A1:AMJ2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="7.08"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="2" style="6" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="6" width="25.42"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="6" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="6" width="22.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="6" width="16.11"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="11" style="6" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="15" width="7.08"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="2" style="15" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="15" width="25.4"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="15" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="15" width="22.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="15" width="16.11"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="11" style="15" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="7" customFormat="true" ht="30.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
+    <row r="1" s="16" customFormat="true" ht="30.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>38</v>
+      <c r="B1" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>139</v>
       </c>
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="n">
+      <c r="A2" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>39</v>
+      <c r="B2" s="15" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add sequences and phylogeny data
</commit_message>
<xml_diff>
--- a/data/lit_review.xlsx
+++ b/data/lit_review.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="227">
   <si>
     <t xml:space="preserve">Reference level</t>
   </si>
@@ -597,7 +597,7 @@
     <t xml:space="preserve">Plasmid-mediated fosA (Tn2921) structure and how it differs from a chromosomally-encoded fosA</t>
   </si>
   <si>
-    <t xml:space="preserve">fosA</t>
+    <t xml:space="preserve">fosA; plasmid-mediated; chromosomally-encoded</t>
   </si>
   <si>
     <t xml:space="preserve">Kieran A. Milner</t>
@@ -1099,6 +1099,467 @@
     <t xml:space="preserve">fosA5; E. coli; fosfomycin resistance</t>
   </si>
   <si>
+    <t xml:space="preserve">Check figure 2 for genetic environment of fosA5</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Plasmid encoded fosfomycin resistance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Falagas fosfomycin review 2010</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Fosfomycin mech of action and res</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Ying Huang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identification of fosA10, a Novel Plasmid-Mediated
+Fosfomycin Resistance Gene of Klebsiella pneumoniae Origin, in Escherichia coli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://doi.org/10.2147/IDR.S251360</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Discovery of novel fosA10 of Kleb origin in E. coli </t>
+  </si>
+  <si>
+    <t xml:space="preserve">fosA10; E. coli; plasmid-mediated </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zachary S. Elliott</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Role of fosA in Challenges with Fosfomycin Susceptibility Testing of Multispecies Klebsiella pneumoniae Carbapenemase-Producing Clinical Isolates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1128/JCM.00634-19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check references 14-19 for fosfomycin AST </t>
+  </si>
+  <si>
+    <t xml:space="preserve">H. Xu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identification of a novel fosfomycin resistance gene (fosA2) in Enterobacter cloacae from the Salmon River, Canada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1111/j.1472-765X.2011.03016.x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Letter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identification of novel fosA2 in Enterobacter cloacae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fosA2; Enterobacter cloacae; fosfomycin resistance; chromosomal</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">- Enterobacter cloacae chromosome contains a 426bp ORF that encodes for FosA, a 141-residue polypeptide with 95% identity to FosA from S. marcescens
+- Strains with FosA2 had a greater resistance to fosfomycin compared to those with FosA
+- fosA2 is chromosomal in E. cloacae but is flanked by Tn2961 therefore has potential of being mobile  and allelic variation in fos</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">R</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> level occurs</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Fosfomycin for treatment of UTIs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ryota Ito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Widespread Fosfomycin Resistance in Gram-Negative Bacteria Attributable to the Chromosomal fosA Gene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1128/mBio.00749-17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acquired vs intrinsic fosA genes in g- bacteria and proposed naming system of plasmid vs chromosomal fosA genes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fosA; plasmid; chromosomal; acquired resistance; intrinsic resistance; gram negative bacteria</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Fosfomycin production by P. syringae</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Susceptibility of isolates to fosfomycin</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Zanna Beharry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Functional Analysis of Active Site Residues of the Fosfomycin Resistance Enzyme FosA from Pseudomonas aeruginosa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1074/jbc.M501052200</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Reference for UTI therapies</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">fos comb therapy S. aureus</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">fos comb therapy P. aeruginosa</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Lynn L. Silver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fosfomycin: Mechanism and Resistance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1101/cshperspect.a025262</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fosfomycin mech of action and resistance </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hyeri Seok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fosfomycin Resistance in Escherichia coli Isolates
+from South Korea and in vitro Activity of Fosfomycin Alone and in Combination with Other Antibiotics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://dx.doi.org/10.3390/antibiotics9030112</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Christopher A. Darlow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amikacin Combined with Fosfomycin for Treatment of Neonatal Sepsis in the Setting of Highly Prevalent Antimicrobial Resistance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1128/AAC.00293-21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matthew E. Falagas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resistance to fosfomycin: Mechanisms, Frequency and Clinical Consequences</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1016/j.ijantimicag.2018.09.013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Annika I. Nilsson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biological Costs and Mechanisms of Fosfomycin Resistance in Escherichia coli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1128/AAC.47.9.2850-2858.2003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thijs ten Doesschate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In vivo acquisition of fosfomycin resistance in Escherichia coli by fosA transmission from commensal flora</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1093/jac/dkz380</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laurent Poirel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identification of FosA8, a Plasmid-Encoded Fosfomycin Resistance Determinant from Escherichia coli, and Its Origin in Leclercia adecarboxylata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1128/AAC.01403-19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shiri Navon-Venezia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Klebsiella pneumoniae: a major worldwide source
+and shuttle for antibiotic resistance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1093/femsre/fux013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K. pneumoniae resistome, plasmids encoding AMR, high risk epidemic clones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K.pneumonia; plasmid; clones; resistome; AMR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Klebsiella pneumonia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IncF plasmids</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kelly L Wyres and Kathryn E Holt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Klebsiella pneumoniae as a key trafficker of drug
+resistance genes from environmental to clinically
+important bacteria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1016/j.mib.2018.04.004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transfer of AMR gene from environmental bacteria to K. pneumo to other bacteria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resistance; genome plasticity; plasmid diversity; ecology</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">CARD AMR database</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Kp plasmids</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Michelle K. Paczosa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Klebsiella pneumoniae: Going on the Offense with a Strong Defense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://dx.doi.org/10.1128/MMBR.00078-15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Types of Kp strains, infections caused by Kp, patient risk factors, Kp virulence factors  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Classical; hypervirulent; pneumonia; liver absesses; resistance; risk factors; virulence factors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check table 1 for HV vs classical Kp, fig 1 summarises the four main virulence factors of Kp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rebekah M. Martin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Colonization, Infection, and the Accessory Genome of Klebsiella pneumoniae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.3389/fcimb.2018.00004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Opportunistic (classical), Hv, and antibiotic res Kp strains, progression from colonisation to infection, colonisation as a reservoir of ABR Kp in hospitals, and the role of the accessory genome in the different types of infections</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antibiotic resistance; opportunistic; hypervirulence; accessory genes; core genome; reservoir; risk factors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Another main reference for virulence factors and Kp AMR resistance
+Check figure 1 for pool of accessory genes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Victoria Ballén</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antibiotic Resistance and Virulence Profiles of Klebsiella pneumoniae Strains Isolated From Different Clinical Sources</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.3389/fcimb.2021.738223</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AMR levels and virulence determinants related to urine, blood, and respiratory samples positive for Kp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antibiotic resistance; hypervirulent; virulence factors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thomas A. Russo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hypervirulent Klebsiella pneumoniae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1128/CMR.00001-19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evolution, epidemiology, structure and function, pathogenesis, risk factors, and infectious sundromes caused by HvKp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check figure 1 for hvKp plasmid schematic</t>
+  </si>
+  <si>
     <t xml:space="preserve">fos gene</t>
   </si>
   <si>
@@ -1124,6 +1585,9 @@
   </si>
   <si>
     <t xml:space="preserve">Shared identity with fosA (%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fosA</t>
   </si>
 </sst>
 </file>
@@ -1191,7 +1655,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1213,7 +1677,13 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFB7B3CA"/>
-        <bgColor rgb="FFCCCCFF"/>
+        <bgColor rgb="FFCCCCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCCC"/>
+        <bgColor rgb="FFB7B3CA"/>
       </patternFill>
     </fill>
   </fills>
@@ -1258,7 +1728,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1307,11 +1777,15 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1361,7 +1835,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FFCCCCCC"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -1458,12 +1932,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ27"/>
+  <dimension ref="A1:AMJ55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="K17" activeCellId="0" sqref="K17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+      <selection pane="bottomLeft" activeCell="L35" activeCellId="0" sqref="L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1478,7 +1952,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="6" width="23.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="6" width="19.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="6" width="16.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="6" width="37.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="7" width="37.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="6" width="28.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="6" width="16.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="6" width="20.3"/>
@@ -1518,7 +1992,7 @@
       <c r="J1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="9" t="s">
         <v>15</v>
       </c>
       <c r="L1" s="8" t="s">
@@ -1570,7 +2044,7 @@
       <c r="J2" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="7" t="s">
         <v>29</v>
       </c>
       <c r="L2" s="6" t="s">
@@ -1668,7 +2142,7 @@
       <c r="J4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="K4" s="7" t="s">
         <v>47</v>
       </c>
       <c r="L4" s="6" t="s">
@@ -1717,6 +2191,7 @@
       <c r="J5" s="6" t="s">
         <v>28</v>
       </c>
+      <c r="K5" s="14"/>
       <c r="L5" s="6" t="s">
         <v>57</v>
       </c>
@@ -1757,6 +2232,7 @@
       <c r="J6" s="6" t="s">
         <v>28</v>
       </c>
+      <c r="K6" s="14"/>
       <c r="M6" s="6" t="s">
         <v>49</v>
       </c>
@@ -1791,7 +2267,7 @@
       <c r="J7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="K7" s="6" t="s">
+      <c r="K7" s="7" t="s">
         <v>67</v>
       </c>
       <c r="L7" s="6" t="s">
@@ -1800,7 +2276,7 @@
       <c r="M7" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="P7" s="14"/>
+      <c r="P7" s="15"/>
     </row>
     <row r="8" customFormat="false" ht="30.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="n">
@@ -1828,13 +2304,14 @@
       <c r="I8" s="6" t="s">
         <v>72</v>
       </c>
+      <c r="K8" s="14"/>
       <c r="M8" s="6" t="s">
         <v>49</v>
       </c>
       <c r="N8" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="P8" s="14"/>
+      <c r="P8" s="15"/>
     </row>
     <row r="9" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="n">
@@ -1868,6 +2345,7 @@
       <c r="J9" s="6" t="s">
         <v>28</v>
       </c>
+      <c r="K9" s="14"/>
       <c r="M9" s="6" t="s">
         <v>49</v>
       </c>
@@ -1899,6 +2377,7 @@
       <c r="J10" s="6" t="s">
         <v>28</v>
       </c>
+      <c r="K10" s="14"/>
       <c r="L10" s="6" t="s">
         <v>82</v>
       </c>
@@ -1908,7 +2387,7 @@
       <c r="N10" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="P10" s="14"/>
+      <c r="P10" s="15"/>
     </row>
     <row r="11" customFormat="false" ht="49.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="n">
@@ -1942,6 +2421,7 @@
       <c r="J11" s="6" t="s">
         <v>28</v>
       </c>
+      <c r="K11" s="14"/>
       <c r="L11" s="6" t="s">
         <v>88</v>
       </c>
@@ -1954,6 +2434,7 @@
       <c r="O11" s="10" t="s">
         <v>90</v>
       </c>
+      <c r="P11" s="13"/>
     </row>
     <row r="12" customFormat="false" ht="30.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="n">
@@ -1987,6 +2468,7 @@
       <c r="J12" s="6" t="s">
         <v>28</v>
       </c>
+      <c r="K12" s="14"/>
       <c r="L12" s="6" t="s">
         <v>96</v>
       </c>
@@ -1995,7 +2477,7 @@
       </c>
       <c r="P12" s="13"/>
     </row>
-    <row r="13" customFormat="false" ht="49.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="n">
         <f aca="false">ROW(A12)</f>
         <v>12</v>
@@ -2027,6 +2509,7 @@
       <c r="J13" s="6" t="s">
         <v>28</v>
       </c>
+      <c r="K13" s="14"/>
       <c r="L13" s="6" t="s">
         <v>102</v>
       </c>
@@ -2073,6 +2556,7 @@
       <c r="J14" s="6" t="s">
         <v>28</v>
       </c>
+      <c r="K14" s="14"/>
       <c r="L14" s="6" t="s">
         <v>110</v>
       </c>
@@ -2119,6 +2603,7 @@
       <c r="J15" s="6" t="s">
         <v>28</v>
       </c>
+      <c r="K15" s="14"/>
       <c r="L15" s="6" t="s">
         <v>117</v>
       </c>
@@ -2165,6 +2650,7 @@
       <c r="J16" s="6" t="s">
         <v>28</v>
       </c>
+      <c r="K16" s="14"/>
       <c r="L16" s="6" t="s">
         <v>124</v>
       </c>
@@ -2211,72 +2697,725 @@
       <c r="J17" s="6" t="s">
         <v>28</v>
       </c>
+      <c r="K17" s="14"/>
+      <c r="L17" s="6" t="s">
+        <v>131</v>
+      </c>
       <c r="M17" s="6" t="s">
         <v>31</v>
       </c>
       <c r="N17" s="6" t="s">
         <v>26</v>
       </c>
+      <c r="O17" s="10" t="s">
+        <v>132</v>
+      </c>
       <c r="P17" s="11"/>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="30.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="n">
         <f aca="false">ROW(A17)</f>
         <v>17</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="D18" s="6" t="n">
+        <v>2020</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K18" s="14"/>
+      <c r="M18" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N18" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="P18" s="11"/>
+    </row>
+    <row r="19" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="n">
         <f aca="false">ROW(A18)</f>
         <v>18</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="D19" s="6" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K19" s="14"/>
+      <c r="L19" s="6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="88.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="n">
         <f aca="false">ROW(A19)</f>
         <v>19</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="D20" s="6" t="n">
+        <v>2011</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K20" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="M20" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N20" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="O20" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="P20" s="11"/>
+    </row>
+    <row r="21" customFormat="false" ht="49.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="n">
         <f aca="false">ROW(A20)</f>
         <v>20</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="D21" s="6" t="n">
+        <v>2017</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K21" s="14"/>
+      <c r="M21" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N21" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="O21" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="P21" s="11"/>
+    </row>
+    <row r="22" customFormat="false" ht="30.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="n">
         <f aca="false">ROW(A21)</f>
         <v>21</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="D22" s="6" t="n">
+        <v>2005</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="K22" s="14"/>
+      <c r="O22" s="10" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="n">
         <f aca="false">ROW(A22)</f>
         <v>22</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="D23" s="6" t="n">
+        <v>2017</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="K23" s="14"/>
+    </row>
+    <row r="24" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="n">
         <f aca="false">ROW(A23)</f>
         <v>23</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="D24" s="6" t="n">
+        <v>2020</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="K24" s="14"/>
+    </row>
+    <row r="25" customFormat="false" ht="30.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="n">
         <f aca="false">ROW(A24)</f>
         <v>24</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="D25" s="6" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="K25" s="14"/>
+    </row>
+    <row r="26" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="n">
         <f aca="false">ROW(A25)</f>
         <v>25</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="D26" s="6" t="n">
+        <v>2018</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="K26" s="14"/>
+    </row>
+    <row r="27" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="n">
         <f aca="false">ROW(A26)</f>
         <v>26</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="D27" s="6" t="n">
+        <v>2003</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="K27" s="14"/>
+    </row>
+    <row r="28" customFormat="false" ht="30.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="6" t="n">
+        <f aca="false">ROW(A27)</f>
+        <v>27</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="D28" s="6" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="K28" s="14"/>
+    </row>
+    <row r="29" customFormat="false" ht="30.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="6" t="n">
+        <f aca="false">ROW(A28)</f>
+        <v>28</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="D29" s="6" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="K29" s="14"/>
+    </row>
+    <row r="30" customFormat="false" ht="30.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="6" t="n">
+        <f aca="false">ROW(A29)</f>
+        <v>29</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="D30" s="6" t="n">
+        <v>2017</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="J30" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K30" s="14"/>
+      <c r="M30" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N30" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="O30" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="P30" s="11"/>
+    </row>
+    <row r="31" customFormat="false" ht="30.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="6" t="n">
+        <f aca="false">ROW(A30)</f>
+        <v>30</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="D31" s="6" t="n">
+        <v>2018</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="J31" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K31" s="14"/>
+      <c r="M31" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N31" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="O31" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="P31" s="11"/>
+    </row>
+    <row r="32" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="6" t="n">
+        <f aca="false">ROW(A31)</f>
+        <v>31</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="D32" s="6" t="n">
+        <v>2016</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H32" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="I32" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="J32" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K32" s="14"/>
+      <c r="L32" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="M32" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N32" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="P32" s="11"/>
+    </row>
+    <row r="33" customFormat="false" ht="79.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="6" t="n">
+        <f aca="false">ROW(A32)</f>
+        <v>32</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="D33" s="6" t="n">
+        <v>2018</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="I33" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="J33" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K33" s="14"/>
+      <c r="L33" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="M33" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N33" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="P33" s="11"/>
+    </row>
+    <row r="34" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="6" t="n">
+        <f aca="false">ROW(A33)</f>
+        <v>33</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="D34" s="6" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="I34" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="J34" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K34" s="14"/>
+      <c r="M34" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N34" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="P34" s="13"/>
+    </row>
+    <row r="35" customFormat="false" ht="49.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="6" t="n">
+        <f aca="false">ROW(A34)</f>
+        <v>34</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="D35" s="6" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="L35" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="O35" s="0"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="6" t="n">
+        <f aca="false">ROW(A35)</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="6" t="n">
+        <f aca="false">ROW(A36)</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="6" t="n">
+        <f aca="false">ROW(A37)</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="6" t="n">
+        <f aca="false">ROW(A38)</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="6" t="n">
+        <f aca="false">ROW(A39)</f>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="6" t="n">
+        <f aca="false">ROW(A40)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="6" t="n">
+        <f aca="false">ROW(A41)</f>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="6" t="n">
+        <f aca="false">ROW(A42)</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="6" t="n">
+        <f aca="false">ROW(A43)</f>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="6" t="n">
+        <f aca="false">ROW(A44)</f>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="6" t="n">
+        <f aca="false">ROW(A45)</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="6" t="n">
+        <f aca="false">ROW(A46)</f>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="6" t="n">
+        <f aca="false">ROW(A47)</f>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="6" t="n">
+        <f aca="false">ROW(A48)</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="6" t="n">
+        <f aca="false">ROW(A49)</f>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="6" t="n">
+        <f aca="false">ROW(A50)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="6" t="n">
+        <f aca="false">ROW(A51)</f>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="6" t="n">
+        <f aca="false">ROW(A52)</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="6" t="n">
+        <f aca="false">ROW(A53)</f>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="6" t="n">
+        <f aca="false">ROW(A54)</f>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -2299,6 +3438,26 @@
     <hyperlink ref="E16" r:id="rId16" display="http://dx.doi.org/10.1128/JCM.01094-14"/>
     <hyperlink ref="O16" r:id="rId17" display="PPF"/>
     <hyperlink ref="E17" r:id="rId18" display="https://doi.org/10.1111/lam.12366"/>
+    <hyperlink ref="E18" r:id="rId19" display="http://doi.org/10.2147/IDR.S251360"/>
+    <hyperlink ref="E19" r:id="rId20" display="https://doi.org/10.1128/JCM.00634-19"/>
+    <hyperlink ref="E20" r:id="rId21" display="https://doi.org/10.1111/j.1472-765X.2011.03016.x"/>
+    <hyperlink ref="O20" r:id="rId22" display="Fosfomycin for treatment of UTIs"/>
+    <hyperlink ref="E21" r:id="rId23" display="https://doi.org/10.1128/mBio.00749-17"/>
+    <hyperlink ref="E22" r:id="rId24" display="https://doi.org/10.1074/jbc.M501052200"/>
+    <hyperlink ref="E23" r:id="rId25" display="https://doi.org/10.1101/cshperspect.a025262"/>
+    <hyperlink ref="E24" r:id="rId26" display="http://dx.doi.org/10.3390/antibiotics9030112"/>
+    <hyperlink ref="E25" r:id="rId27" display="https://doi.org/10.1128/AAC.00293-21"/>
+    <hyperlink ref="E26" r:id="rId28" display="https://doi.org/10.1016/j.ijantimicag.2018.09.013"/>
+    <hyperlink ref="E27" r:id="rId29" display="https://doi.org/10.1128/AAC.47.9.2850-2858.2003"/>
+    <hyperlink ref="E28" r:id="rId30" display="https://doi.org/10.1093/jac/dkz380"/>
+    <hyperlink ref="E29" r:id="rId31" display="https://doi.org/10.1128/AAC.01403-19"/>
+    <hyperlink ref="E30" r:id="rId32" display="https://doi.org/10.1093/femsre/fux013"/>
+    <hyperlink ref="O30" r:id="rId33" display="IncF plasmids"/>
+    <hyperlink ref="E31" r:id="rId34" display="https://doi.org/10.1016/j.mib.2018.04.004"/>
+    <hyperlink ref="E32" r:id="rId35" display="http://dx.doi.org/10.1128/MMBR.00078-15"/>
+    <hyperlink ref="E33" r:id="rId36" display="https://doi.org/10.3389/fcimb.2018.00004"/>
+    <hyperlink ref="E34" r:id="rId37" display="https://doi.org/10.3389/fcimb.2021.738223"/>
+    <hyperlink ref="E35" r:id="rId38" display="https://doi.org/10.1128/CMR.00001-19"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2323,54 +3482,54 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="15" width="7.08"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="2" style="15" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="15" width="25.4"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="15" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="15" width="22.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="15" width="16.11"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="11" style="15" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="16" width="7.08"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="2" style="16" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="16" width="25.4"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="16" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="16" width="22.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="16" width="16.11"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="11" style="16" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="16" customFormat="true" ht="30.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="16" t="s">
+    <row r="1" s="17" customFormat="true" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="G1" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="H1" s="16" t="s">
-        <v>137</v>
-      </c>
-      <c r="I1" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="J1" s="16" t="s">
-        <v>139</v>
+      <c r="B1" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>225</v>
       </c>
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="15" t="n">
+      <c r="A2" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>77</v>
+      <c r="B2" s="16" t="s">
+        <v>226</v>
       </c>
     </row>
   </sheetData>

</xml_diff>